<commit_message>
Change radio to choice for forms demo (make online compatible)
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/Experiments/BigFiveInventory/bigFiveItems.xlsx
+++ b/psychopy/demos/builder/Experiments/BigFiveInventory/bigFiveItems.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\BigFiveInventory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\44797\PycharmProjects\psychopy\psychopy\demos\builder\Experiments\BigFiveInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CBF0F7-382E-4229-B550-C83ABF085D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D472144-3D9A-4C7E-9A7C-D7882BEB1962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -559,7 +559,7 @@
     <t>horiz</t>
   </si>
   <si>
-    <t>radio</t>
+    <t>choice</t>
   </si>
 </sst>
 </file>
@@ -979,24 +979,24 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
-    <col min="5" max="6" width="25.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" style="2" customWidth="1"/>
-    <col min="8" max="11" width="15.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="1" max="1" width="6.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" style="2" customWidth="1"/>
+    <col min="8" max="11" width="15.7265625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.1796875" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.1796875" style="4" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1376,7 +1376,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1905,7 +1905,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>

</xml_diff>